<commit_message>
Halted produtiction for now
</commit_message>
<xml_diff>
--- a/SemanaOperativa/output.xlsx
+++ b/SemanaOperativa/output.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="ago a nov" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>10/08</t>
   </si>
@@ -85,13 +85,13 @@
     <t>Grande</t>
   </si>
   <si>
-    <t>Iguaçu</t>
+    <t>IguaÃ§u</t>
   </si>
   <si>
     <t>Itabapoana</t>
   </si>
   <si>
-    <t>Jacuí</t>
+    <t>JacuÃ­</t>
   </si>
   <si>
     <t>Paraguai</t>
@@ -100,52 +100,41 @@
     <t>Paranapanema</t>
   </si>
   <si>
-    <t>Paranaíba</t>
-  </si>
-  <si>
-    <t>Paraná</t>
-  </si>
-  <si>
-    <t>Paraíba do Sul</t>
-  </si>
-  <si>
-    <t>Parnaíba</t>
-  </si>
-  <si>
-    <t>São Francisco</t>
+    <t>ParanaÃ­ba</t>
+  </si>
+  <si>
+    <t>ParanÃ¡</t>
+  </si>
+  <si>
+    <t>ParaÃ­ba do Sul</t>
+  </si>
+  <si>
+    <t>ParnaÃ­ba</t>
+  </si>
+  <si>
+    <t>SÃ£o Francisco</t>
   </si>
   <si>
     <t>Taquari Antas</t>
   </si>
   <si>
-    <t>Tietê</t>
+    <t>TietÃª</t>
   </si>
   <si>
     <t>Tocantins</t>
   </si>
   <si>
     <t>Uruguai</t>
-  </si>
-  <si>
-    <t>Cell A1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,18 +148,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF193B4F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -200,12 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -509,91 +489,89 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
         <v>8</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1">
         <v>9</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1">
         <v>10</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1">
         <v>11</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4">
@@ -649,7 +627,7 @@
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B5">
@@ -705,7 +683,7 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B6">
@@ -761,7 +739,7 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B7">
@@ -817,7 +795,7 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8">
@@ -873,7 +851,7 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B9">
@@ -929,7 +907,7 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10">
@@ -985,7 +963,7 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B11">
@@ -1041,7 +1019,7 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B12">
@@ -1097,7 +1075,7 @@
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B13">
@@ -1153,7 +1131,7 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B14">
@@ -1209,7 +1187,7 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15">
@@ -1265,7 +1243,7 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B16">
@@ -1321,7 +1299,7 @@
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17">
@@ -1377,7 +1355,7 @@
       </c>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B18">
@@ -1433,7 +1411,7 @@
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B19">
@@ -1489,7 +1467,7 @@
       </c>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B20">
@@ -1545,7 +1523,7 @@
       </c>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B21">
@@ -1601,7 +1579,7 @@
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B22">
@@ -1657,7 +1635,7 @@
       </c>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B23">

</xml_diff>